<commit_message>
Fixed minor bugs and optimised committed
</commit_message>
<xml_diff>
--- a/AEF_template/AEF_CMA6_second_iteration.unmerged.xlsx
+++ b/AEF_template/AEF_CMA6_second_iteration.unmerged.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unfccc365.sharepoint.com/sites/Mitigation/Paris Agreement Article 6/Article 6.2/03_CARP/consistency/AEF_template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="35" documentId="13_ncr:1_{0B9CFA14-F56A-4387-990D-A503B02D9DCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E04AF5F0-DCE4-4A45-8A3F-4B506EEDF4D6}"/>
+  <xr:revisionPtr revIDLastSave="45" documentId="13_ncr:1_{0B9CFA14-F56A-4387-990D-A503B02D9DCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EB637992-6077-9744-9380-9FC651B37D96}"/>
   <bookViews>
-    <workbookView xWindow="23860" yWindow="700" windowWidth="26760" windowHeight="22960" tabRatio="618" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6640" yWindow="840" windowWidth="26760" windowHeight="22960" tabRatio="618" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="5" r:id="rId1"/>
@@ -694,6 +694,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
+  </numFmts>
   <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -973,7 +977,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="105">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1023,9 +1027,6 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1180,6 +1181,48 @@
     <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1200,6 +1243,9 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1593,7 +1639,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E3F6B9B-E1BC-4D08-AE97-F15181187A83}">
   <dimension ref="B1:C104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B52" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView topLeftCell="B66" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="B53" sqref="A53:XFD53"/>
     </sheetView>
   </sheetViews>
@@ -1632,74 +1678,74 @@
       </c>
     </row>
     <row r="6" spans="2:3" ht="16" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="74" t="s">
+      <c r="B6" s="73" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="75" t="s">
+      <c r="C6" s="74" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B7" s="74" t="s">
+      <c r="B7" s="73" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="75" t="s">
+      <c r="C7" s="74" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="8" spans="2:3" ht="28" x14ac:dyDescent="0.2">
-      <c r="B8" s="74" t="s">
+      <c r="B8" s="73" t="s">
         <v>90</v>
       </c>
-      <c r="C8" s="75" t="s">
+      <c r="C8" s="74" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B9" s="74" t="s">
+      <c r="B9" s="73" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="75" t="s">
+      <c r="C9" s="74" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="10" spans="2:3" ht="28" x14ac:dyDescent="0.2">
-      <c r="B10" s="74" t="s">
+      <c r="B10" s="73" t="s">
         <v>98</v>
       </c>
-      <c r="C10" s="75" t="s">
+      <c r="C10" s="74" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="11" spans="2:3" ht="28" x14ac:dyDescent="0.2">
-      <c r="B11" s="74" t="s">
+      <c r="B11" s="73" t="s">
         <v>99</v>
       </c>
-      <c r="C11" s="75" t="s">
+      <c r="C11" s="74" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B12" s="74" t="s">
+      <c r="B12" s="73" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="75" t="s">
+      <c r="C12" s="74" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B13" s="74" t="s">
+      <c r="B13" s="73" t="s">
         <v>27</v>
       </c>
-      <c r="C13" s="75" t="s">
+      <c r="C13" s="74" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="14" spans="2:3" ht="43" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="78" t="s">
+      <c r="B14" s="77" t="s">
         <v>101</v>
       </c>
-      <c r="C14" s="79" t="s">
+      <c r="C14" s="78" t="s">
         <v>125</v>
       </c>
     </row>
@@ -1718,154 +1764,154 @@
       </c>
     </row>
     <row r="20" spans="2:3" ht="16" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="74" t="s">
+      <c r="B20" s="73" t="s">
         <v>28</v>
       </c>
-      <c r="C20" s="75" t="s">
+      <c r="C20" s="74" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B21" s="74" t="s">
+      <c r="B21" s="73" t="s">
         <v>29</v>
       </c>
-      <c r="C21" s="75" t="s">
+      <c r="C21" s="74" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B22" s="74" t="s">
+      <c r="B22" s="73" t="s">
         <v>67</v>
       </c>
-      <c r="C22" s="75" t="s">
+      <c r="C22" s="74" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B23" s="74" t="s">
+      <c r="B23" s="73" t="s">
         <v>31</v>
       </c>
-      <c r="C23" s="75" t="s">
+      <c r="C23" s="74" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="24" spans="2:3" ht="28" x14ac:dyDescent="0.2">
-      <c r="B24" s="74" t="s">
+      <c r="B24" s="73" t="s">
         <v>76</v>
       </c>
-      <c r="C24" s="75" t="s">
+      <c r="C24" s="74" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B25" s="74" t="s">
+      <c r="B25" s="73" t="s">
         <v>32</v>
       </c>
-      <c r="C25" s="75" t="s">
+      <c r="C25" s="74" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="26" spans="2:3" ht="46" x14ac:dyDescent="0.2">
-      <c r="B26" s="74" t="s">
+      <c r="B26" s="73" t="s">
         <v>110</v>
       </c>
-      <c r="C26" s="75" t="s">
+      <c r="C26" s="74" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="27" spans="2:3" ht="42" x14ac:dyDescent="0.2">
-      <c r="B27" s="74" t="s">
+      <c r="B27" s="73" t="s">
         <v>71</v>
       </c>
-      <c r="C27" s="75" t="s">
+      <c r="C27" s="74" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="28" spans="2:3" ht="28" x14ac:dyDescent="0.2">
-      <c r="B28" s="74" t="s">
+      <c r="B28" s="73" t="s">
         <v>33</v>
       </c>
-      <c r="C28" s="75" t="s">
+      <c r="C28" s="74" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B29" s="74" t="s">
+      <c r="B29" s="73" t="s">
         <v>35</v>
       </c>
-      <c r="C29" s="75" t="s">
+      <c r="C29" s="74" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B30" s="74" t="s">
+      <c r="B30" s="73" t="s">
         <v>37</v>
       </c>
-      <c r="C30" s="75" t="s">
+      <c r="C30" s="74" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="31" spans="2:3" ht="42" x14ac:dyDescent="0.2">
-      <c r="B31" s="74" t="s">
+      <c r="B31" s="73" t="s">
         <v>105</v>
       </c>
-      <c r="C31" s="75" t="s">
+      <c r="C31" s="74" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="32" spans="2:3" ht="28" x14ac:dyDescent="0.2">
-      <c r="B32" s="74" t="s">
+      <c r="B32" s="73" t="s">
         <v>106</v>
       </c>
-      <c r="C32" s="75" t="s">
+      <c r="C32" s="74" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="33" spans="2:3" ht="70" x14ac:dyDescent="0.2">
-      <c r="B33" s="74" t="s">
+      <c r="B33" s="73" t="s">
         <v>38</v>
       </c>
-      <c r="C33" s="75" t="s">
+      <c r="C33" s="74" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="34" spans="2:3" ht="56" x14ac:dyDescent="0.2">
-      <c r="B34" s="74" t="s">
+      <c r="B34" s="73" t="s">
         <v>107</v>
       </c>
-      <c r="C34" s="75" t="s">
+      <c r="C34" s="74" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="35" spans="2:3" ht="28" x14ac:dyDescent="0.2">
-      <c r="B35" s="74" t="s">
+      <c r="B35" s="73" t="s">
         <v>108</v>
       </c>
-      <c r="C35" s="75" t="s">
+      <c r="C35" s="74" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="36" spans="2:3" ht="28" x14ac:dyDescent="0.2">
-      <c r="B36" s="74" t="s">
+      <c r="B36" s="73" t="s">
         <v>39</v>
       </c>
-      <c r="C36" s="75" t="s">
+      <c r="C36" s="74" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="37" spans="2:3" ht="56" x14ac:dyDescent="0.2">
-      <c r="B37" s="74" t="s">
+      <c r="B37" s="73" t="s">
         <v>52</v>
       </c>
-      <c r="C37" s="75" t="s">
+      <c r="C37" s="74" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="38" spans="2:3" ht="29" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="76" t="s">
+      <c r="B38" s="75" t="s">
         <v>94</v>
       </c>
-      <c r="C38" s="77" t="s">
+      <c r="C38" s="76" t="s">
         <v>138</v>
       </c>
     </row>
@@ -1883,218 +1929,218 @@
       </c>
     </row>
     <row r="43" spans="2:3" ht="16" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B43" s="74" t="s">
+      <c r="B43" s="73" t="s">
         <v>46</v>
       </c>
-      <c r="C43" s="75" t="s">
+      <c r="C43" s="74" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="44" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B44" s="80" t="s">
+      <c r="B44" s="79" t="s">
         <v>10</v>
       </c>
-      <c r="C44" s="81" t="s">
+      <c r="C44" s="80" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="45" spans="2:3" ht="20.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B45" s="80" t="s">
+      <c r="B45" s="79" t="s">
         <v>146</v>
       </c>
-      <c r="C45" s="81" t="s">
+      <c r="C45" s="80" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="46" spans="2:3" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B46" s="74" t="s">
+      <c r="B46" s="73" t="s">
         <v>67</v>
       </c>
-      <c r="C46" s="75" t="s">
+      <c r="C46" s="74" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="47" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B47" s="74" t="s">
+      <c r="B47" s="73" t="s">
         <v>28</v>
       </c>
-      <c r="C47" s="75" t="s">
+      <c r="C47" s="74" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="48" spans="2:3" ht="28" x14ac:dyDescent="0.2">
-      <c r="B48" s="74" t="s">
+      <c r="B48" s="73" t="s">
         <v>92</v>
       </c>
-      <c r="C48" s="75" t="s">
+      <c r="C48" s="74" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="49" spans="2:3" ht="28" x14ac:dyDescent="0.2">
-      <c r="B49" s="74" t="s">
+      <c r="B49" s="73" t="s">
         <v>68</v>
       </c>
-      <c r="C49" s="75" t="s">
+      <c r="C49" s="74" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="50" spans="2:3" ht="28" x14ac:dyDescent="0.2">
-      <c r="B50" s="74" t="s">
+      <c r="B50" s="73" t="s">
         <v>69</v>
       </c>
-      <c r="C50" s="75" t="s">
+      <c r="C50" s="74" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="51" spans="2:3" ht="28" x14ac:dyDescent="0.2">
-      <c r="B51" s="74" t="s">
+      <c r="B51" s="73" t="s">
         <v>70</v>
       </c>
-      <c r="C51" s="75" t="s">
+      <c r="C51" s="74" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="52" spans="2:3" ht="56" x14ac:dyDescent="0.2">
-      <c r="B52" s="74" t="s">
+      <c r="B52" s="73" t="s">
         <v>66</v>
       </c>
-      <c r="C52" s="75" t="s">
+      <c r="C52" s="74" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="53" spans="2:3" ht="56" x14ac:dyDescent="0.2">
-      <c r="B53" s="74" t="s">
+      <c r="B53" s="73" t="s">
         <v>116</v>
       </c>
-      <c r="C53" s="75" t="s">
+      <c r="C53" s="74" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="54" spans="2:3" ht="56" x14ac:dyDescent="0.2">
-      <c r="B54" s="74" t="s">
+      <c r="B54" s="73" t="s">
         <v>117</v>
       </c>
-      <c r="C54" s="75" t="s">
+      <c r="C54" s="74" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="55" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B55" s="74" t="s">
+      <c r="B55" s="73" t="s">
         <v>32</v>
       </c>
-      <c r="C55" s="75" t="s">
+      <c r="C55" s="74" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="56" spans="2:3" ht="46" x14ac:dyDescent="0.2">
-      <c r="B56" s="74" t="s">
+      <c r="B56" s="73" t="s">
         <v>110</v>
       </c>
-      <c r="C56" s="75" t="s">
+      <c r="C56" s="74" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="57" spans="2:3" ht="42" x14ac:dyDescent="0.2">
-      <c r="B57" s="74" t="s">
+      <c r="B57" s="73" t="s">
         <v>71</v>
       </c>
-      <c r="C57" s="75" t="s">
+      <c r="C57" s="74" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="58" spans="2:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="B58" s="74" t="s">
+      <c r="B58" s="73" t="s">
         <v>140</v>
       </c>
-      <c r="C58" s="75" t="s">
+      <c r="C58" s="74" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="59" spans="2:3" ht="28" x14ac:dyDescent="0.2">
-      <c r="B59" s="74" t="s">
+      <c r="B59" s="73" t="s">
         <v>112</v>
       </c>
-      <c r="C59" s="75" t="s">
+      <c r="C59" s="74" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="60" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B60" s="74" t="s">
+      <c r="B60" s="73" t="s">
         <v>44</v>
       </c>
-      <c r="C60" s="75" t="s">
+      <c r="C60" s="74" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="61" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B61" s="74" t="s">
+      <c r="B61" s="73" t="s">
         <v>45</v>
       </c>
-      <c r="C61" s="75" t="s">
+      <c r="C61" s="74" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="62" spans="2:3" ht="70" x14ac:dyDescent="0.2">
-      <c r="B62" s="74" t="s">
+      <c r="B62" s="73" t="s">
         <v>93</v>
       </c>
-      <c r="C62" s="75" t="s">
+      <c r="C62" s="74" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="63" spans="2:3" ht="70" x14ac:dyDescent="0.2">
-      <c r="B63" s="74" t="s">
+      <c r="B63" s="73" t="s">
         <v>72</v>
       </c>
-      <c r="C63" s="75" t="s">
+      <c r="C63" s="74" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="64" spans="2:3" ht="84" x14ac:dyDescent="0.2">
-      <c r="B64" s="74" t="s">
+      <c r="B64" s="73" t="s">
         <v>114</v>
       </c>
-      <c r="C64" s="75" t="s">
+      <c r="C64" s="74" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="65" spans="2:3" ht="56" x14ac:dyDescent="0.2">
-      <c r="B65" s="74" t="s">
+      <c r="B65" s="73" t="s">
         <v>118</v>
       </c>
-      <c r="C65" s="75" t="s">
+      <c r="C65" s="74" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="66" spans="2:3" ht="56" x14ac:dyDescent="0.2">
-      <c r="B66" s="74" t="s">
+      <c r="B66" s="73" t="s">
         <v>91</v>
       </c>
-      <c r="C66" s="75" t="s">
+      <c r="C66" s="74" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="67" spans="2:3" ht="42" x14ac:dyDescent="0.2">
-      <c r="B67" s="74" t="s">
+      <c r="B67" s="73" t="s">
         <v>115</v>
       </c>
-      <c r="C67" s="75" t="s">
+      <c r="C67" s="74" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="68" spans="2:3" ht="42" x14ac:dyDescent="0.2">
-      <c r="B68" s="74" t="s">
+      <c r="B68" s="73" t="s">
         <v>119</v>
       </c>
-      <c r="C68" s="75" t="s">
+      <c r="C68" s="74" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="69" spans="2:3" ht="29" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B69" s="76" t="s">
+      <c r="B69" s="75" t="s">
         <v>94</v>
       </c>
-      <c r="C69" s="77" t="s">
+      <c r="C69" s="76" t="s">
         <v>138</v>
       </c>
     </row>
@@ -2112,130 +2158,130 @@
       </c>
     </row>
     <row r="75" spans="2:3" ht="16" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B75" s="74" t="s">
+      <c r="B75" s="73" t="s">
         <v>67</v>
       </c>
-      <c r="C75" s="75" t="s">
+      <c r="C75" s="74" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="76" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B76" s="74" t="s">
+      <c r="B76" s="73" t="s">
         <v>28</v>
       </c>
-      <c r="C76" s="75" t="s">
+      <c r="C76" s="74" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="77" spans="2:3" ht="28" x14ac:dyDescent="0.2">
-      <c r="B77" s="74" t="s">
+      <c r="B77" s="73" t="s">
         <v>92</v>
       </c>
-      <c r="C77" s="75" t="s">
+      <c r="C77" s="74" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="78" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B78" s="74" t="s">
+      <c r="B78" s="73" t="s">
         <v>68</v>
       </c>
-      <c r="C78" s="75" t="s">
+      <c r="C78" s="74" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="79" spans="2:3" ht="28" x14ac:dyDescent="0.2">
-      <c r="B79" s="74" t="s">
+      <c r="B79" s="73" t="s">
         <v>69</v>
       </c>
-      <c r="C79" s="75" t="s">
+      <c r="C79" s="74" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="80" spans="2:3" ht="28" x14ac:dyDescent="0.2">
-      <c r="B80" s="74" t="s">
+      <c r="B80" s="73" t="s">
         <v>70</v>
       </c>
-      <c r="C80" s="75" t="s">
+      <c r="C80" s="74" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="81" spans="2:3" ht="56" x14ac:dyDescent="0.2">
-      <c r="B81" s="74" t="s">
+      <c r="B81" s="73" t="s">
         <v>66</v>
       </c>
-      <c r="C81" s="75" t="s">
+      <c r="C81" s="74" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="82" spans="2:3" ht="56" x14ac:dyDescent="0.2">
-      <c r="B82" s="74" t="s">
+      <c r="B82" s="73" t="s">
         <v>116</v>
       </c>
-      <c r="C82" s="75" t="s">
+      <c r="C82" s="74" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="83" spans="2:3" ht="56" x14ac:dyDescent="0.2">
-      <c r="B83" s="74" t="s">
+      <c r="B83" s="73" t="s">
         <v>117</v>
       </c>
-      <c r="C83" s="75" t="s">
+      <c r="C83" s="74" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="84" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B84" s="74" t="s">
+      <c r="B84" s="73" t="s">
         <v>32</v>
       </c>
-      <c r="C84" s="75" t="s">
+      <c r="C84" s="74" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="85" spans="2:3" ht="42" x14ac:dyDescent="0.2">
-      <c r="B85" s="74" t="s">
+      <c r="B85" s="73" t="s">
         <v>110</v>
       </c>
-      <c r="C85" s="75" t="s">
+      <c r="C85" s="74" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="86" spans="2:3" ht="42" x14ac:dyDescent="0.2">
-      <c r="B86" s="74" t="s">
+      <c r="B86" s="73" t="s">
         <v>71</v>
       </c>
-      <c r="C86" s="75" t="s">
+      <c r="C86" s="74" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="87" spans="2:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="B87" s="74" t="s">
+      <c r="B87" s="73" t="s">
         <v>147</v>
       </c>
-      <c r="C87" s="75" t="s">
+      <c r="C87" s="74" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="88" spans="2:3" ht="28" x14ac:dyDescent="0.2">
-      <c r="B88" s="74" t="s">
+      <c r="B88" s="73" t="s">
         <v>112</v>
       </c>
-      <c r="C88" s="75" t="s">
+      <c r="C88" s="74" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="89" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B89" s="74" t="s">
+      <c r="B89" s="73" t="s">
         <v>44</v>
       </c>
-      <c r="C89" s="75" t="s">
+      <c r="C89" s="74" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="90" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B90" s="76" t="s">
+      <c r="B90" s="75" t="s">
         <v>45</v>
       </c>
-      <c r="C90" s="77" t="s">
+      <c r="C90" s="76" t="s">
         <v>73</v>
       </c>
     </row>
@@ -2309,10 +2355,10 @@
       </c>
     </row>
     <row r="103" spans="2:3" ht="29" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B103" s="76" t="s">
+      <c r="B103" s="75" t="s">
         <v>94</v>
       </c>
-      <c r="C103" s="77" t="s">
+      <c r="C103" s="76" t="s">
         <v>138</v>
       </c>
     </row>
@@ -2329,8 +2375,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:C13"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2359,7 +2405,7 @@
       <c r="B5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="104" t="s">
         <v>49</v>
       </c>
     </row>
@@ -2375,7 +2421,7 @@
       <c r="B7" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="81" t="s">
         <v>159</v>
       </c>
     </row>
@@ -2383,7 +2429,7 @@
       <c r="B8" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="C8" s="59" t="s">
+      <c r="C8" s="58" t="s">
         <v>153</v>
       </c>
     </row>
@@ -2391,7 +2437,7 @@
       <c r="B9" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="C9" s="59" t="s">
+      <c r="C9" s="58" t="s">
         <v>153</v>
       </c>
     </row>
@@ -2412,16 +2458,16 @@
       </c>
     </row>
     <row r="12" spans="2:3" ht="29" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="61" t="s">
+      <c r="B12" s="60" t="s">
         <v>101</v>
       </c>
-      <c r="C12" s="60" t="s">
+      <c r="C12" s="59" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="13" spans="2:3" ht="16" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="82"/>
-      <c r="C13" s="82"/>
+      <c r="B13" s="97"/>
+      <c r="C13" s="97"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2437,14 +2483,14 @@
   <dimension ref="B3:U14"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="U10" sqref="U10"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8.83203125" style="15"/>
     <col min="2" max="2" width="9.83203125" style="15" customWidth="1"/>
-    <col min="3" max="3" width="10" style="15" customWidth="1"/>
+    <col min="3" max="3" width="10" style="82" customWidth="1"/>
     <col min="4" max="4" width="8.83203125" style="15"/>
     <col min="5" max="5" width="11" style="15" customWidth="1"/>
     <col min="6" max="6" width="3.1640625" style="15" customWidth="1"/>
@@ -2473,58 +2519,58 @@
       </c>
     </row>
     <row r="5" spans="2:21" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="83" t="s">
+      <c r="B5" s="98" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="83"/>
-      <c r="D5" s="83"/>
-      <c r="E5" s="83"/>
-      <c r="F5" s="34"/>
-      <c r="G5" s="35" t="s">
+      <c r="C5" s="98"/>
+      <c r="D5" s="98"/>
+      <c r="E5" s="98"/>
+      <c r="F5" s="33"/>
+      <c r="G5" s="34" t="s">
         <v>51</v>
       </c>
-      <c r="H5" s="32"/>
-      <c r="I5" s="32"/>
-      <c r="J5" s="32"/>
-      <c r="K5" s="32"/>
-      <c r="L5" s="32"/>
-      <c r="M5" s="32"/>
-      <c r="N5" s="32"/>
-      <c r="O5" s="32"/>
-      <c r="P5" s="32"/>
-      <c r="Q5" s="32"/>
-      <c r="R5" s="32"/>
-      <c r="S5" s="32"/>
-      <c r="T5" s="53"/>
-      <c r="U5" s="53"/>
+      <c r="H5" s="31"/>
+      <c r="I5" s="31"/>
+      <c r="J5" s="31"/>
+      <c r="K5" s="31"/>
+      <c r="L5" s="31"/>
+      <c r="M5" s="31"/>
+      <c r="N5" s="31"/>
+      <c r="O5" s="31"/>
+      <c r="P5" s="31"/>
+      <c r="Q5" s="31"/>
+      <c r="R5" s="31"/>
+      <c r="S5" s="31"/>
+      <c r="T5" s="52"/>
+      <c r="U5" s="52"/>
     </row>
     <row r="6" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B6" s="39"/>
-      <c r="C6" s="39"/>
-      <c r="D6" s="39"/>
-      <c r="E6" s="39"/>
-      <c r="F6" s="39"/>
-      <c r="G6" s="34"/>
-      <c r="H6" s="37"/>
-      <c r="I6" s="37"/>
-      <c r="J6" s="37"/>
-      <c r="K6" s="33"/>
-      <c r="L6" s="33"/>
-      <c r="M6" s="33"/>
-      <c r="N6" s="33"/>
-      <c r="O6" s="33"/>
-      <c r="P6" s="33"/>
-      <c r="Q6" s="33"/>
-      <c r="R6" s="33"/>
-      <c r="S6" s="33"/>
-      <c r="T6" s="63"/>
-      <c r="U6" s="63"/>
+      <c r="B6" s="38"/>
+      <c r="C6" s="83"/>
+      <c r="D6" s="38"/>
+      <c r="E6" s="38"/>
+      <c r="F6" s="38"/>
+      <c r="G6" s="33"/>
+      <c r="H6" s="36"/>
+      <c r="I6" s="36"/>
+      <c r="J6" s="36"/>
+      <c r="K6" s="32"/>
+      <c r="L6" s="32"/>
+      <c r="M6" s="32"/>
+      <c r="N6" s="32"/>
+      <c r="O6" s="32"/>
+      <c r="P6" s="32"/>
+      <c r="Q6" s="32"/>
+      <c r="R6" s="32"/>
+      <c r="S6" s="32"/>
+      <c r="T6" s="62"/>
+      <c r="U6" s="62"/>
     </row>
     <row r="7" spans="2:21" ht="28.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B7" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="21" t="s">
+      <c r="C7" s="84" t="s">
         <v>29</v>
       </c>
       <c r="D7" s="21" t="s">
@@ -2540,7 +2586,7 @@
       <c r="H7" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="I7" s="62" t="s">
+      <c r="I7" s="61" t="s">
         <v>110</v>
       </c>
       <c r="J7" s="21" t="s">
@@ -2567,126 +2613,126 @@
       <c r="Q7" s="21" t="s">
         <v>107</v>
       </c>
-      <c r="R7" s="62" t="s">
+      <c r="R7" s="61" t="s">
         <v>108</v>
       </c>
       <c r="S7" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="T7" s="64" t="s">
+      <c r="T7" s="63" t="s">
         <v>52</v>
       </c>
-      <c r="U7" s="64" t="s">
+      <c r="U7" s="63" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="8" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B8" s="19"/>
-      <c r="C8" s="23"/>
-      <c r="D8" s="24"/>
-      <c r="E8" s="24"/>
-      <c r="F8" s="24"/>
-      <c r="G8" s="24"/>
+      <c r="C8" s="85"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="23"/>
       <c r="H8" s="19" t="s">
         <v>53</v>
       </c>
       <c r="I8" s="19"/>
       <c r="J8" s="19"/>
-      <c r="K8" s="25"/>
-      <c r="L8" s="25"/>
-      <c r="M8" s="25" t="s">
+      <c r="K8" s="24"/>
+      <c r="L8" s="24"/>
+      <c r="M8" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="N8" s="25"/>
+      <c r="N8" s="24"/>
       <c r="O8" s="19"/>
       <c r="P8" s="19"/>
       <c r="Q8" s="19"/>
       <c r="R8" s="19"/>
-      <c r="S8" s="58"/>
-      <c r="T8" s="25" t="s">
+      <c r="S8" s="57"/>
+      <c r="T8" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="U8" s="25"/>
+      <c r="U8" s="24"/>
     </row>
     <row r="9" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B9" s="19"/>
-      <c r="C9" s="24"/>
-      <c r="D9" s="24"/>
-      <c r="E9" s="24"/>
-      <c r="F9" s="24"/>
-      <c r="G9" s="24"/>
+      <c r="C9" s="86"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="23"/>
+      <c r="G9" s="23"/>
       <c r="H9" s="19" t="s">
         <v>55</v>
       </c>
       <c r="I9" s="19"/>
       <c r="J9" s="19"/>
-      <c r="K9" s="25"/>
-      <c r="L9" s="25"/>
-      <c r="M9" s="25" t="s">
+      <c r="K9" s="24"/>
+      <c r="L9" s="24"/>
+      <c r="M9" s="24" t="s">
         <v>102</v>
       </c>
-      <c r="N9" s="25"/>
+      <c r="N9" s="24"/>
       <c r="O9" s="19"/>
       <c r="P9" s="19"/>
       <c r="Q9" s="19"/>
       <c r="R9" s="19"/>
       <c r="S9" s="19"/>
-      <c r="T9" s="25" t="s">
+      <c r="T9" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="U9" s="25"/>
+      <c r="U9" s="24"/>
     </row>
     <row r="10" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B10" s="19"/>
-      <c r="C10" s="24"/>
-      <c r="D10" s="24"/>
-      <c r="E10" s="24"/>
-      <c r="F10" s="24"/>
-      <c r="G10" s="24"/>
+      <c r="C10" s="86"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="23"/>
+      <c r="G10" s="23"/>
       <c r="H10" s="19"/>
       <c r="I10" s="19"/>
       <c r="J10" s="19"/>
-      <c r="K10" s="25"/>
-      <c r="L10" s="25"/>
-      <c r="M10" s="25" t="s">
+      <c r="K10" s="24"/>
+      <c r="L10" s="24"/>
+      <c r="M10" s="24" t="s">
         <v>103</v>
       </c>
-      <c r="N10" s="25"/>
+      <c r="N10" s="24"/>
       <c r="O10" s="19"/>
       <c r="P10" s="19"/>
       <c r="Q10" s="19"/>
       <c r="R10" s="19"/>
       <c r="S10" s="19"/>
-      <c r="T10" s="25" t="s">
+      <c r="T10" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="U10" s="25"/>
+      <c r="U10" s="24"/>
     </row>
     <row r="11" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B11" s="19"/>
-      <c r="C11" s="19"/>
+      <c r="C11" s="87"/>
       <c r="D11" s="19"/>
       <c r="E11" s="19"/>
       <c r="F11" s="19"/>
       <c r="G11" s="19"/>
       <c r="I11" s="19"/>
       <c r="J11" s="19"/>
-      <c r="K11" s="25"/>
-      <c r="L11" s="25"/>
-      <c r="M11" s="25" t="s">
+      <c r="K11" s="24"/>
+      <c r="L11" s="24"/>
+      <c r="M11" s="24" t="s">
         <v>104</v>
       </c>
-      <c r="N11" s="25"/>
+      <c r="N11" s="24"/>
       <c r="O11" s="19"/>
       <c r="P11" s="19"/>
       <c r="Q11" s="19"/>
       <c r="R11" s="19"/>
       <c r="S11" s="19"/>
-      <c r="U11" s="25"/>
+      <c r="U11" s="24"/>
     </row>
     <row r="12" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B12" s="19"/>
-      <c r="C12" s="19"/>
+      <c r="C12" s="87"/>
       <c r="D12" s="19"/>
       <c r="E12" s="19"/>
       <c r="F12" s="19"/>
@@ -2694,22 +2740,22 @@
       <c r="H12" s="19"/>
       <c r="I12" s="19"/>
       <c r="J12" s="19"/>
-      <c r="K12" s="25"/>
-      <c r="L12" s="25"/>
-      <c r="M12" s="25" t="s">
+      <c r="K12" s="24"/>
+      <c r="L12" s="24"/>
+      <c r="M12" s="24" t="s">
         <v>95</v>
       </c>
-      <c r="N12" s="25"/>
+      <c r="N12" s="24"/>
       <c r="O12" s="19"/>
       <c r="P12" s="19"/>
       <c r="Q12" s="19"/>
       <c r="R12" s="19"/>
-      <c r="S12" s="57"/>
-      <c r="U12" s="25"/>
+      <c r="S12" s="56"/>
+      <c r="U12" s="24"/>
     </row>
     <row r="13" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B13" s="19"/>
-      <c r="C13" s="19"/>
+      <c r="C13" s="87"/>
       <c r="D13" s="19"/>
       <c r="E13" s="19"/>
       <c r="F13" s="19"/>
@@ -2717,43 +2763,43 @@
       <c r="H13" s="19"/>
       <c r="I13" s="19"/>
       <c r="J13" s="19"/>
-      <c r="K13" s="25"/>
-      <c r="L13" s="25"/>
-      <c r="M13" s="25" t="s">
+      <c r="K13" s="24"/>
+      <c r="L13" s="24"/>
+      <c r="M13" s="24" t="s">
         <v>96</v>
       </c>
-      <c r="N13" s="25"/>
+      <c r="N13" s="24"/>
       <c r="O13" s="19"/>
       <c r="P13" s="19"/>
       <c r="Q13" s="19"/>
       <c r="R13" s="19"/>
       <c r="S13" s="19"/>
-      <c r="T13" s="25"/>
-      <c r="U13" s="25"/>
+      <c r="T13" s="24"/>
+      <c r="U13" s="24"/>
     </row>
     <row r="14" spans="2:21" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="26"/>
-      <c r="C14" s="26"/>
-      <c r="D14" s="26"/>
-      <c r="E14" s="26"/>
-      <c r="F14" s="26"/>
-      <c r="G14" s="26"/>
-      <c r="H14" s="26"/>
-      <c r="I14" s="26"/>
-      <c r="J14" s="26"/>
-      <c r="K14" s="26"/>
-      <c r="L14" s="26"/>
-      <c r="M14" s="26" t="s">
+      <c r="B14" s="25"/>
+      <c r="C14" s="88"/>
+      <c r="D14" s="25"/>
+      <c r="E14" s="25"/>
+      <c r="F14" s="25"/>
+      <c r="G14" s="25"/>
+      <c r="H14" s="25"/>
+      <c r="I14" s="25"/>
+      <c r="J14" s="25"/>
+      <c r="K14" s="25"/>
+      <c r="L14" s="25"/>
+      <c r="M14" s="25" t="s">
         <v>97</v>
       </c>
-      <c r="N14" s="26"/>
-      <c r="O14" s="26"/>
-      <c r="P14" s="26"/>
-      <c r="Q14" s="26"/>
-      <c r="R14" s="26"/>
-      <c r="S14" s="26"/>
-      <c r="T14" s="26"/>
-      <c r="U14" s="26"/>
+      <c r="N14" s="25"/>
+      <c r="O14" s="25"/>
+      <c r="P14" s="25"/>
+      <c r="Q14" s="25"/>
+      <c r="R14" s="25"/>
+      <c r="S14" s="25"/>
+      <c r="T14" s="25"/>
+      <c r="U14" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2768,14 +2814,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{903CFF46-A00D-4851-8A69-F36031122945}">
   <dimension ref="B3:AH13"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="AF8" sqref="AF8"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8.83203125" style="15"/>
-    <col min="2" max="2" width="8.1640625" style="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.1640625" style="82" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.1640625" style="15" customWidth="1"/>
     <col min="4" max="4" width="17.1640625" style="15" customWidth="1"/>
     <col min="5" max="5" width="15.1640625" style="15" bestFit="1" customWidth="1"/>
@@ -2809,179 +2855,179 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:34" x14ac:dyDescent="0.2">
-      <c r="B3" s="27" t="s">
+      <c r="B3" s="89" t="s">
         <v>40</v>
       </c>
-      <c r="C3" s="27"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
     </row>
     <row r="4" spans="2:34" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="29" t="s">
+      <c r="B4" s="90" t="s">
         <v>75</v>
       </c>
-      <c r="C4" s="30"/>
-      <c r="D4" s="30"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="32" t="s">
+      <c r="C4" s="29"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="31" t="s">
         <v>58</v>
       </c>
       <c r="G4" s="20"/>
-      <c r="H4" s="31"/>
-      <c r="I4" s="32"/>
-      <c r="J4" s="32"/>
-      <c r="K4" s="32"/>
-      <c r="L4" s="32"/>
-      <c r="M4" s="32"/>
-      <c r="N4" s="32"/>
-      <c r="O4" s="32"/>
-      <c r="P4" s="32"/>
-      <c r="Q4" s="32"/>
-      <c r="R4" s="32"/>
-      <c r="S4" s="32"/>
-      <c r="T4" s="32"/>
+      <c r="H4" s="30"/>
+      <c r="I4" s="31"/>
+      <c r="J4" s="31"/>
+      <c r="K4" s="31"/>
+      <c r="L4" s="31"/>
+      <c r="M4" s="31"/>
+      <c r="N4" s="31"/>
+      <c r="O4" s="31"/>
+      <c r="P4" s="31"/>
+      <c r="Q4" s="31"/>
+      <c r="R4" s="31"/>
+      <c r="S4" s="31"/>
+      <c r="T4" s="31"/>
       <c r="U4" s="20"/>
-      <c r="V4" s="33"/>
-      <c r="W4" s="33"/>
-      <c r="X4" s="34"/>
-      <c r="Y4" s="35" t="s">
+      <c r="V4" s="32"/>
+      <c r="W4" s="32"/>
+      <c r="X4" s="33"/>
+      <c r="Y4" s="34" t="s">
         <v>78</v>
       </c>
-      <c r="Z4" s="35"/>
-      <c r="AA4" s="35"/>
-      <c r="AB4" s="35"/>
-      <c r="AC4" s="35"/>
-      <c r="AD4" s="35"/>
-      <c r="AE4" s="35"/>
-      <c r="AF4" s="34"/>
-      <c r="AG4" s="52"/>
-      <c r="AH4" s="52"/>
+      <c r="Z4" s="34"/>
+      <c r="AA4" s="34"/>
+      <c r="AB4" s="34"/>
+      <c r="AC4" s="34"/>
+      <c r="AD4" s="34"/>
+      <c r="AE4" s="34"/>
+      <c r="AF4" s="33"/>
+      <c r="AG4" s="51"/>
+      <c r="AH4" s="51"/>
     </row>
     <row r="5" spans="2:34" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E5" s="24"/>
-      <c r="F5" s="32"/>
-      <c r="G5" s="66"/>
-      <c r="H5" s="32" t="s">
+      <c r="E5" s="23"/>
+      <c r="F5" s="31"/>
+      <c r="G5" s="65"/>
+      <c r="H5" s="31" t="s">
         <v>59</v>
       </c>
-      <c r="I5" s="32"/>
-      <c r="J5" s="32"/>
-      <c r="K5" s="36"/>
-      <c r="L5" s="32"/>
-      <c r="M5" s="36"/>
-      <c r="N5" s="36"/>
+      <c r="I5" s="31"/>
+      <c r="J5" s="31"/>
+      <c r="K5" s="35"/>
+      <c r="L5" s="31"/>
+      <c r="M5" s="35"/>
+      <c r="N5" s="35"/>
       <c r="O5" s="18"/>
-      <c r="P5" s="30" t="s">
+      <c r="P5" s="29" t="s">
         <v>60</v>
       </c>
-      <c r="Q5" s="30"/>
-      <c r="R5" s="30"/>
-      <c r="S5" s="30"/>
-      <c r="T5" s="30"/>
+      <c r="Q5" s="29"/>
+      <c r="R5" s="29"/>
+      <c r="S5" s="29"/>
+      <c r="T5" s="29"/>
       <c r="U5" s="18"/>
       <c r="V5" s="20" t="s">
         <v>61</v>
       </c>
       <c r="W5" s="20"/>
-      <c r="X5" s="37"/>
-      <c r="Y5" s="29" t="s">
+      <c r="X5" s="36"/>
+      <c r="Y5" s="28" t="s">
         <v>79</v>
       </c>
-      <c r="Z5" s="29"/>
-      <c r="AA5" s="29"/>
-      <c r="AB5" s="29"/>
-      <c r="AC5" s="29"/>
-      <c r="AD5" s="29"/>
-      <c r="AE5" s="29"/>
-      <c r="AF5" s="37"/>
-      <c r="AG5" s="24"/>
-      <c r="AH5" s="24"/>
+      <c r="Z5" s="28"/>
+      <c r="AA5" s="28"/>
+      <c r="AB5" s="28"/>
+      <c r="AC5" s="28"/>
+      <c r="AD5" s="28"/>
+      <c r="AE5" s="28"/>
+      <c r="AF5" s="36"/>
+      <c r="AG5" s="23"/>
+      <c r="AH5" s="23"/>
     </row>
     <row r="6" spans="2:34" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="24"/>
-      <c r="C6" s="39"/>
-      <c r="D6" s="39"/>
-      <c r="E6" s="24"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="39"/>
-      <c r="H6" s="39"/>
-      <c r="I6" s="53"/>
-      <c r="J6" s="53"/>
+      <c r="B6" s="86"/>
+      <c r="C6" s="38"/>
+      <c r="D6" s="38"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="38"/>
+      <c r="H6" s="38"/>
+      <c r="I6" s="52"/>
+      <c r="J6" s="52"/>
       <c r="K6" s="18"/>
-      <c r="L6" s="29" t="s">
+      <c r="L6" s="28" t="s">
         <v>62</v>
       </c>
-      <c r="M6" s="29"/>
-      <c r="N6" s="29"/>
+      <c r="M6" s="28"/>
+      <c r="N6" s="28"/>
       <c r="O6" s="18"/>
-      <c r="P6" s="39"/>
-      <c r="Q6" s="39"/>
-      <c r="R6" s="39"/>
-      <c r="S6" s="39"/>
-      <c r="T6" s="39"/>
+      <c r="P6" s="38"/>
+      <c r="Q6" s="38"/>
+      <c r="R6" s="38"/>
+      <c r="S6" s="38"/>
+      <c r="T6" s="38"/>
       <c r="U6" s="18"/>
-      <c r="V6" s="39"/>
-      <c r="W6" s="39"/>
-      <c r="X6" s="37"/>
-      <c r="Y6" s="85" t="s">
+      <c r="V6" s="38"/>
+      <c r="W6" s="38"/>
+      <c r="X6" s="36"/>
+      <c r="Y6" s="100" t="s">
         <v>113</v>
       </c>
-      <c r="Z6" s="85"/>
-      <c r="AA6" s="41"/>
-      <c r="AB6" s="84" t="s">
+      <c r="Z6" s="100"/>
+      <c r="AA6" s="40"/>
+      <c r="AB6" s="99" t="s">
         <v>57</v>
       </c>
-      <c r="AC6" s="84"/>
-      <c r="AD6" s="84"/>
-      <c r="AE6" s="84"/>
-      <c r="AF6" s="37"/>
-      <c r="AG6" s="24"/>
-      <c r="AH6" s="24"/>
+      <c r="AC6" s="99"/>
+      <c r="AD6" s="99"/>
+      <c r="AE6" s="99"/>
+      <c r="AF6" s="36"/>
+      <c r="AG6" s="23"/>
+      <c r="AH6" s="23"/>
     </row>
     <row r="7" spans="2:34" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="24"/>
-      <c r="C7" s="39"/>
-      <c r="D7" s="39"/>
-      <c r="E7" s="24"/>
-      <c r="F7" s="24"/>
-      <c r="G7" s="39"/>
-      <c r="H7" s="39"/>
-      <c r="I7" s="40" t="s">
+      <c r="B7" s="86"/>
+      <c r="C7" s="38"/>
+      <c r="D7" s="38"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="38"/>
+      <c r="H7" s="38"/>
+      <c r="I7" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="J7" s="40"/>
+      <c r="J7" s="39"/>
       <c r="K7" s="18"/>
-      <c r="L7" s="24"/>
-      <c r="M7" s="29" t="s">
+      <c r="L7" s="23"/>
+      <c r="M7" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="N7" s="36"/>
+      <c r="N7" s="35"/>
       <c r="O7" s="18"/>
-      <c r="P7" s="39"/>
-      <c r="Q7" s="39"/>
-      <c r="R7" s="39"/>
-      <c r="S7" s="39"/>
-      <c r="T7" s="39"/>
+      <c r="P7" s="38"/>
+      <c r="Q7" s="38"/>
+      <c r="R7" s="38"/>
+      <c r="S7" s="38"/>
+      <c r="T7" s="38"/>
       <c r="U7" s="18"/>
-      <c r="V7" s="39"/>
-      <c r="W7" s="39"/>
-      <c r="X7" s="37"/>
-      <c r="Y7" s="41"/>
-      <c r="Z7" s="41"/>
-      <c r="AA7" s="41"/>
-      <c r="AB7" s="24"/>
-      <c r="AC7" s="24"/>
-      <c r="AD7" s="24"/>
-      <c r="AE7" s="24"/>
-      <c r="AF7" s="37"/>
-      <c r="AG7" s="24"/>
-      <c r="AH7" s="24"/>
+      <c r="V7" s="38"/>
+      <c r="W7" s="38"/>
+      <c r="X7" s="36"/>
+      <c r="Y7" s="40"/>
+      <c r="Z7" s="40"/>
+      <c r="AA7" s="40"/>
+      <c r="AB7" s="23"/>
+      <c r="AC7" s="23"/>
+      <c r="AD7" s="23"/>
+      <c r="AE7" s="23"/>
+      <c r="AF7" s="36"/>
+      <c r="AG7" s="23"/>
+      <c r="AH7" s="23"/>
     </row>
     <row r="8" spans="2:34" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="21" t="s">
+      <c r="B8" s="84" t="s">
         <v>46</v>
       </c>
-      <c r="C8" s="62" t="s">
+      <c r="C8" s="61" t="s">
         <v>10</v>
       </c>
       <c r="D8" s="21" t="s">
@@ -2999,23 +3045,23 @@
       <c r="H8" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="I8" s="42" t="s">
+      <c r="I8" s="41" t="s">
         <v>69</v>
       </c>
-      <c r="J8" s="42" t="s">
+      <c r="J8" s="41" t="s">
         <v>70</v>
       </c>
-      <c r="K8" s="43"/>
-      <c r="L8" s="44" t="s">
+      <c r="K8" s="42"/>
+      <c r="L8" s="43" t="s">
         <v>66</v>
       </c>
-      <c r="M8" s="42" t="s">
+      <c r="M8" s="41" t="s">
         <v>116</v>
       </c>
-      <c r="N8" s="42" t="s">
+      <c r="N8" s="41" t="s">
         <v>117</v>
       </c>
-      <c r="O8" s="43"/>
+      <c r="O8" s="42"/>
       <c r="P8" s="21" t="s">
         <v>32</v>
       </c>
@@ -3031,7 +3077,7 @@
       <c r="T8" s="21" t="s">
         <v>112</v>
       </c>
-      <c r="U8" s="43"/>
+      <c r="U8" s="42"/>
       <c r="V8" s="21" t="s">
         <v>44</v>
       </c>
@@ -3067,23 +3113,23 @@
       </c>
     </row>
     <row r="9" spans="2:34" ht="28" x14ac:dyDescent="0.2">
-      <c r="B9" s="45"/>
-      <c r="C9" s="25" t="s">
+      <c r="B9" s="91"/>
+      <c r="C9" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="25"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="25"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="24"/>
+      <c r="F9" s="24"/>
       <c r="G9" s="19"/>
-      <c r="H9" s="25"/>
-      <c r="I9" s="25"/>
-      <c r="J9" s="46"/>
+      <c r="H9" s="24"/>
+      <c r="I9" s="24"/>
+      <c r="J9" s="45"/>
       <c r="K9" s="19"/>
       <c r="L9" s="19"/>
       <c r="M9" s="19"/>
       <c r="N9" s="19"/>
       <c r="O9" s="19"/>
-      <c r="P9" s="25" t="s">
+      <c r="P9" s="24" t="s">
         <v>53</v>
       </c>
       <c r="Q9" s="19"/>
@@ -3091,38 +3137,38 @@
       <c r="S9" s="19"/>
       <c r="T9" s="19"/>
       <c r="U9" s="19"/>
-      <c r="V9" s="25" t="s">
+      <c r="V9" s="24" t="s">
         <v>65</v>
       </c>
       <c r="W9" s="19"/>
       <c r="X9" s="19"/>
-      <c r="Y9" s="47"/>
-      <c r="Z9" s="47"/>
-      <c r="AA9" s="47"/>
-      <c r="AB9" s="25"/>
-      <c r="AC9" s="45"/>
-      <c r="AD9" s="45"/>
-      <c r="AE9" s="45"/>
+      <c r="Y9" s="46"/>
+      <c r="Z9" s="46"/>
+      <c r="AA9" s="46"/>
+      <c r="AB9" s="24"/>
+      <c r="AC9" s="44"/>
+      <c r="AD9" s="44"/>
+      <c r="AE9" s="44"/>
       <c r="AF9" s="19"/>
     </row>
     <row r="10" spans="2:34" x14ac:dyDescent="0.2">
-      <c r="B10" s="45"/>
-      <c r="C10" s="25" t="s">
+      <c r="B10" s="91"/>
+      <c r="C10" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="25"/>
-      <c r="E10" s="25"/>
-      <c r="F10" s="25"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="24"/>
+      <c r="F10" s="24"/>
       <c r="G10" s="19"/>
-      <c r="H10" s="25"/>
-      <c r="I10" s="25"/>
-      <c r="J10" s="46"/>
+      <c r="H10" s="24"/>
+      <c r="I10" s="24"/>
+      <c r="J10" s="45"/>
       <c r="K10" s="19"/>
       <c r="L10" s="19"/>
       <c r="M10" s="19"/>
       <c r="N10" s="19"/>
       <c r="O10" s="19"/>
-      <c r="P10" s="25" t="s">
+      <c r="P10" s="24" t="s">
         <v>63</v>
       </c>
       <c r="Q10" s="19"/>
@@ -3130,64 +3176,64 @@
       <c r="S10" s="19"/>
       <c r="T10" s="19"/>
       <c r="U10" s="19"/>
-      <c r="V10" s="25" t="s">
+      <c r="V10" s="24" t="s">
         <v>64</v>
       </c>
       <c r="W10" s="19"/>
       <c r="X10" s="19"/>
-      <c r="Y10" s="47"/>
-      <c r="Z10" s="47"/>
-      <c r="AA10" s="47"/>
-      <c r="AB10" s="25"/>
-      <c r="AC10" s="45"/>
-      <c r="AD10" s="45"/>
-      <c r="AE10" s="45"/>
+      <c r="Y10" s="46"/>
+      <c r="Z10" s="46"/>
+      <c r="AA10" s="46"/>
+      <c r="AB10" s="24"/>
+      <c r="AC10" s="44"/>
+      <c r="AD10" s="44"/>
+      <c r="AE10" s="44"/>
       <c r="AF10" s="19"/>
     </row>
     <row r="11" spans="2:34" x14ac:dyDescent="0.2">
-      <c r="B11" s="45"/>
-      <c r="C11" s="25" t="s">
+      <c r="B11" s="91"/>
+      <c r="C11" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="25"/>
-      <c r="E11" s="25"/>
-      <c r="F11" s="25"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="24"/>
       <c r="G11" s="19"/>
-      <c r="H11" s="25"/>
-      <c r="I11" s="25"/>
-      <c r="J11" s="46"/>
+      <c r="H11" s="24"/>
+      <c r="I11" s="24"/>
+      <c r="J11" s="45"/>
       <c r="K11" s="19"/>
       <c r="M11" s="19"/>
       <c r="N11" s="19"/>
       <c r="O11" s="19"/>
-      <c r="P11" s="57"/>
+      <c r="P11" s="56"/>
       <c r="R11" s="19"/>
       <c r="S11" s="19"/>
       <c r="T11" s="19"/>
       <c r="U11" s="19"/>
       <c r="W11" s="19"/>
       <c r="X11" s="19"/>
-      <c r="Y11" s="47"/>
-      <c r="Z11" s="47"/>
-      <c r="AA11" s="47"/>
-      <c r="AB11" s="58"/>
-      <c r="AC11" s="45"/>
-      <c r="AD11" s="45"/>
-      <c r="AE11" s="45"/>
+      <c r="Y11" s="46"/>
+      <c r="Z11" s="46"/>
+      <c r="AA11" s="46"/>
+      <c r="AB11" s="57"/>
+      <c r="AC11" s="44"/>
+      <c r="AD11" s="44"/>
+      <c r="AE11" s="44"/>
       <c r="AF11" s="19"/>
     </row>
     <row r="12" spans="2:34" x14ac:dyDescent="0.2">
-      <c r="B12" s="45"/>
-      <c r="C12" s="25" t="s">
+      <c r="B12" s="91"/>
+      <c r="C12" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="25"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="25"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="24"/>
       <c r="G12" s="19"/>
-      <c r="H12" s="25"/>
-      <c r="I12" s="25"/>
-      <c r="J12" s="46"/>
+      <c r="H12" s="24"/>
+      <c r="I12" s="24"/>
+      <c r="J12" s="45"/>
       <c r="K12" s="19"/>
       <c r="M12" s="19"/>
       <c r="N12" s="19"/>
@@ -3201,29 +3247,29 @@
       <c r="V12" s="19"/>
       <c r="W12" s="19"/>
       <c r="X12" s="19"/>
-      <c r="Y12" s="47"/>
-      <c r="Z12" s="47"/>
-      <c r="AA12" s="47"/>
-      <c r="AB12" s="47"/>
-      <c r="AC12" s="45"/>
-      <c r="AD12" s="45"/>
-      <c r="AE12" s="45"/>
+      <c r="Y12" s="46"/>
+      <c r="Z12" s="46"/>
+      <c r="AA12" s="46"/>
+      <c r="AB12" s="46"/>
+      <c r="AC12" s="44"/>
+      <c r="AD12" s="44"/>
+      <c r="AE12" s="44"/>
       <c r="AF12" s="19"/>
     </row>
     <row r="13" spans="2:34" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="71"/>
-      <c r="C13" s="26" t="s">
+      <c r="B13" s="92"/>
+      <c r="C13" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="D13" s="26"/>
-      <c r="E13" s="72"/>
-      <c r="F13" s="72"/>
+      <c r="D13" s="25"/>
+      <c r="E13" s="71"/>
+      <c r="F13" s="71"/>
       <c r="G13" s="12"/>
-      <c r="H13" s="72"/>
-      <c r="I13" s="72"/>
-      <c r="J13" s="50"/>
+      <c r="H13" s="71"/>
+      <c r="I13" s="71"/>
+      <c r="J13" s="49"/>
       <c r="K13" s="12"/>
-      <c r="L13" s="51"/>
+      <c r="L13" s="50"/>
       <c r="M13" s="12"/>
       <c r="N13" s="12"/>
       <c r="O13" s="12"/>
@@ -3236,16 +3282,16 @@
       <c r="V13" s="12"/>
       <c r="W13" s="12"/>
       <c r="X13" s="12"/>
-      <c r="Y13" s="73"/>
-      <c r="Z13" s="73"/>
-      <c r="AA13" s="73"/>
-      <c r="AB13" s="73"/>
-      <c r="AC13" s="71"/>
-      <c r="AD13" s="71"/>
-      <c r="AE13" s="71"/>
+      <c r="Y13" s="72"/>
+      <c r="Z13" s="72"/>
+      <c r="AA13" s="72"/>
+      <c r="AB13" s="72"/>
+      <c r="AC13" s="70"/>
+      <c r="AD13" s="70"/>
+      <c r="AE13" s="70"/>
       <c r="AF13" s="12"/>
-      <c r="AG13" s="51"/>
-      <c r="AH13" s="51"/>
+      <c r="AG13" s="50"/>
+      <c r="AH13" s="50"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -3262,7 +3308,7 @@
   <dimension ref="B3:U34"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T7" sqref="T7"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3290,105 +3336,105 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:21" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="87" t="s">
+      <c r="B3" s="102" t="s">
         <v>47</v>
       </c>
-      <c r="C3" s="87"/>
-      <c r="D3" s="87"/>
-      <c r="E3" s="87"/>
-      <c r="F3" s="87"/>
-      <c r="G3" s="87"/>
-      <c r="H3" s="87"/>
-      <c r="I3" s="87"/>
-      <c r="J3" s="87"/>
-      <c r="K3" s="87"/>
-      <c r="L3" s="51"/>
-      <c r="M3" s="88"/>
-      <c r="N3" s="88"/>
-      <c r="O3" s="88"/>
-      <c r="P3" s="88"/>
-      <c r="Q3" s="88"/>
-      <c r="R3" s="88"/>
-      <c r="S3" s="88"/>
-      <c r="T3" s="88"/>
+      <c r="C3" s="102"/>
+      <c r="D3" s="102"/>
+      <c r="E3" s="102"/>
+      <c r="F3" s="102"/>
+      <c r="G3" s="102"/>
+      <c r="H3" s="102"/>
+      <c r="I3" s="102"/>
+      <c r="J3" s="102"/>
+      <c r="K3" s="102"/>
+      <c r="L3" s="50"/>
+      <c r="M3" s="103"/>
+      <c r="N3" s="103"/>
+      <c r="O3" s="103"/>
+      <c r="P3" s="103"/>
+      <c r="Q3" s="103"/>
+      <c r="R3" s="103"/>
+      <c r="S3" s="103"/>
+      <c r="T3" s="103"/>
     </row>
     <row r="4" spans="2:21" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="67"/>
-      <c r="C4" s="68"/>
-      <c r="D4" s="69"/>
-      <c r="E4" s="68"/>
-      <c r="F4" s="86" t="s">
+      <c r="B4" s="66"/>
+      <c r="C4" s="67"/>
+      <c r="D4" s="68"/>
+      <c r="E4" s="67"/>
+      <c r="F4" s="101" t="s">
         <v>59</v>
       </c>
-      <c r="G4" s="86"/>
-      <c r="H4" s="86"/>
-      <c r="I4" s="86"/>
-      <c r="J4" s="86"/>
-      <c r="K4" s="86"/>
-      <c r="L4" s="70"/>
-      <c r="M4" s="86" t="s">
+      <c r="G4" s="101"/>
+      <c r="H4" s="101"/>
+      <c r="I4" s="101"/>
+      <c r="J4" s="101"/>
+      <c r="K4" s="101"/>
+      <c r="L4" s="69"/>
+      <c r="M4" s="101" t="s">
         <v>60</v>
       </c>
-      <c r="N4" s="86"/>
-      <c r="O4" s="86"/>
-      <c r="P4" s="86"/>
-      <c r="Q4" s="86"/>
-      <c r="R4" s="70"/>
-      <c r="S4" s="86" t="s">
+      <c r="N4" s="101"/>
+      <c r="O4" s="101"/>
+      <c r="P4" s="101"/>
+      <c r="Q4" s="101"/>
+      <c r="R4" s="69"/>
+      <c r="S4" s="101" t="s">
         <v>61</v>
       </c>
-      <c r="T4" s="86"/>
-      <c r="U4" s="37"/>
+      <c r="T4" s="101"/>
+      <c r="U4" s="36"/>
     </row>
     <row r="5" spans="2:21" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="65"/>
-      <c r="C5" s="24"/>
-      <c r="D5" s="39"/>
-      <c r="E5" s="39"/>
-      <c r="F5" s="84" t="s">
+      <c r="B5" s="64"/>
+      <c r="C5" s="23"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="38"/>
+      <c r="F5" s="99" t="s">
         <v>42</v>
       </c>
-      <c r="G5" s="84"/>
+      <c r="G5" s="99"/>
       <c r="H5" s="18"/>
-      <c r="I5" s="84" t="s">
+      <c r="I5" s="99" t="s">
         <v>62</v>
       </c>
-      <c r="J5" s="84"/>
-      <c r="K5" s="84"/>
+      <c r="J5" s="99"/>
+      <c r="K5" s="99"/>
       <c r="L5" s="18"/>
-      <c r="M5" s="39"/>
-      <c r="N5" s="39"/>
-      <c r="O5" s="39"/>
-      <c r="P5" s="39"/>
-      <c r="Q5" s="39"/>
+      <c r="M5" s="38"/>
+      <c r="N5" s="38"/>
+      <c r="O5" s="38"/>
+      <c r="P5" s="38"/>
+      <c r="Q5" s="38"/>
       <c r="R5" s="18"/>
-      <c r="S5" s="39"/>
-      <c r="T5" s="39"/>
-      <c r="U5" s="37"/>
+      <c r="S5" s="38"/>
+      <c r="T5" s="38"/>
+      <c r="U5" s="36"/>
     </row>
     <row r="6" spans="2:21" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="65"/>
-      <c r="C6" s="24"/>
-      <c r="D6" s="39"/>
-      <c r="E6" s="39"/>
-      <c r="F6" s="38"/>
-      <c r="G6" s="38"/>
+      <c r="B6" s="64"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="38"/>
+      <c r="E6" s="38"/>
+      <c r="F6" s="37"/>
+      <c r="G6" s="37"/>
       <c r="H6" s="18"/>
-      <c r="I6" s="24"/>
-      <c r="J6" s="84" t="s">
+      <c r="I6" s="23"/>
+      <c r="J6" s="99" t="s">
         <v>43</v>
       </c>
-      <c r="K6" s="84"/>
+      <c r="K6" s="99"/>
       <c r="L6" s="18"/>
-      <c r="M6" s="39"/>
-      <c r="N6" s="39"/>
-      <c r="O6" s="39"/>
-      <c r="P6" s="39"/>
-      <c r="Q6" s="39"/>
+      <c r="M6" s="38"/>
+      <c r="N6" s="38"/>
+      <c r="O6" s="38"/>
+      <c r="P6" s="38"/>
+      <c r="Q6" s="38"/>
       <c r="R6" s="18"/>
-      <c r="S6" s="39"/>
-      <c r="T6" s="39"/>
-      <c r="U6" s="37"/>
+      <c r="S6" s="38"/>
+      <c r="T6" s="38"/>
+      <c r="U6" s="36"/>
     </row>
     <row r="7" spans="2:21" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B7" s="21" t="s">
@@ -3400,26 +3446,26 @@
       <c r="D7" s="21" t="s">
         <v>92</v>
       </c>
-      <c r="E7" s="62" t="s">
+      <c r="E7" s="61" t="s">
         <v>68</v>
       </c>
-      <c r="F7" s="42" t="s">
+      <c r="F7" s="41" t="s">
         <v>69</v>
       </c>
-      <c r="G7" s="42" t="s">
+      <c r="G7" s="41" t="s">
         <v>70</v>
       </c>
-      <c r="H7" s="43"/>
+      <c r="H7" s="42"/>
       <c r="I7" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="J7" s="42" t="s">
+      <c r="J7" s="41" t="s">
         <v>116</v>
       </c>
-      <c r="K7" s="42" t="s">
+      <c r="K7" s="41" t="s">
         <v>117</v>
       </c>
-      <c r="L7" s="43"/>
+      <c r="L7" s="42"/>
       <c r="M7" s="21" t="s">
         <v>32</v>
       </c>
@@ -3435,7 +3481,7 @@
       <c r="Q7" s="21" t="s">
         <v>112</v>
       </c>
-      <c r="R7" s="43"/>
+      <c r="R7" s="42"/>
       <c r="S7" s="21" t="s">
         <v>44</v>
       </c>
@@ -3445,12 +3491,12 @@
       <c r="U7" s="21"/>
     </row>
     <row r="8" spans="2:21" ht="28" x14ac:dyDescent="0.2">
-      <c r="B8" s="25"/>
-      <c r="C8" s="25"/>
+      <c r="B8" s="24"/>
+      <c r="C8" s="24"/>
       <c r="D8" s="19"/>
-      <c r="E8" s="25"/>
-      <c r="F8" s="25"/>
-      <c r="G8" s="46"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="45"/>
       <c r="H8" s="19"/>
       <c r="I8" s="19"/>
       <c r="J8" s="19"/>
@@ -3464,19 +3510,19 @@
       <c r="P8" s="19"/>
       <c r="Q8" s="19"/>
       <c r="R8" s="19"/>
-      <c r="S8" s="25" t="s">
+      <c r="S8" s="24" t="s">
         <v>65</v>
       </c>
       <c r="T8" s="19"/>
       <c r="U8" s="19"/>
     </row>
     <row r="9" spans="2:21" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="26"/>
-      <c r="C9" s="26"/>
+      <c r="B9" s="25"/>
+      <c r="C9" s="25"/>
       <c r="D9" s="12"/>
-      <c r="E9" s="26"/>
-      <c r="F9" s="26"/>
-      <c r="G9" s="50"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="25"/>
+      <c r="G9" s="49"/>
       <c r="H9" s="12"/>
       <c r="I9" s="12"/>
       <c r="J9" s="12"/>
@@ -3490,19 +3536,19 @@
       <c r="P9" s="12"/>
       <c r="Q9" s="12"/>
       <c r="R9" s="12"/>
-      <c r="S9" s="26" t="s">
+      <c r="S9" s="25" t="s">
         <v>64</v>
       </c>
       <c r="T9" s="12"/>
       <c r="U9" s="12"/>
     </row>
     <row r="10" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B10" s="25"/>
-      <c r="C10" s="25"/>
+      <c r="B10" s="24"/>
+      <c r="C10" s="24"/>
       <c r="D10" s="19"/>
-      <c r="E10" s="25"/>
-      <c r="F10" s="25"/>
-      <c r="G10" s="46"/>
+      <c r="E10" s="24"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="45"/>
       <c r="H10" s="19"/>
       <c r="J10" s="19"/>
       <c r="K10" s="19"/>
@@ -3515,12 +3561,12 @@
       <c r="U10" s="19"/>
     </row>
     <row r="11" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B11" s="25"/>
-      <c r="C11" s="25"/>
+      <c r="B11" s="24"/>
+      <c r="C11" s="24"/>
       <c r="D11" s="19"/>
-      <c r="E11" s="25"/>
-      <c r="F11" s="25"/>
-      <c r="G11" s="46"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="45"/>
       <c r="H11" s="19"/>
       <c r="J11" s="19"/>
       <c r="K11" s="19"/>
@@ -3536,14 +3582,14 @@
       <c r="U11" s="19"/>
     </row>
     <row r="12" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B12" s="25"/>
-      <c r="C12" s="25"/>
+      <c r="B12" s="24"/>
+      <c r="C12" s="24"/>
       <c r="D12" s="19"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="25"/>
-      <c r="G12" s="46"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="24"/>
+      <c r="G12" s="45"/>
       <c r="H12" s="19"/>
-      <c r="I12" s="46"/>
+      <c r="I12" s="45"/>
       <c r="J12" s="19"/>
       <c r="K12" s="19"/>
       <c r="L12" s="19"/>
@@ -3558,12 +3604,12 @@
       <c r="U12" s="19"/>
     </row>
     <row r="13" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B13" s="48"/>
-      <c r="C13" s="48"/>
+      <c r="B13" s="47"/>
+      <c r="C13" s="47"/>
       <c r="D13" s="19"/>
-      <c r="E13" s="48"/>
-      <c r="F13" s="48"/>
-      <c r="G13" s="46"/>
+      <c r="E13" s="47"/>
+      <c r="F13" s="47"/>
+      <c r="G13" s="45"/>
       <c r="H13" s="19"/>
       <c r="J13" s="19"/>
       <c r="K13" s="19"/>
@@ -3579,12 +3625,12 @@
       <c r="U13" s="19"/>
     </row>
     <row r="14" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B14" s="48"/>
-      <c r="C14" s="48"/>
+      <c r="B14" s="47"/>
+      <c r="C14" s="47"/>
       <c r="D14" s="19"/>
-      <c r="E14" s="48"/>
-      <c r="F14" s="48"/>
-      <c r="G14" s="46"/>
+      <c r="E14" s="47"/>
+      <c r="F14" s="47"/>
+      <c r="G14" s="45"/>
       <c r="H14" s="19"/>
       <c r="J14" s="19"/>
       <c r="K14" s="19"/>
@@ -3600,12 +3646,12 @@
       <c r="U14" s="19"/>
     </row>
     <row r="15" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B15" s="48"/>
-      <c r="C15" s="48"/>
+      <c r="B15" s="47"/>
+      <c r="C15" s="47"/>
       <c r="D15" s="19"/>
-      <c r="E15" s="48"/>
-      <c r="F15" s="48"/>
-      <c r="G15" s="46"/>
+      <c r="E15" s="47"/>
+      <c r="F15" s="47"/>
+      <c r="G15" s="45"/>
       <c r="H15" s="19"/>
       <c r="J15" s="19"/>
       <c r="K15" s="19"/>
@@ -3621,12 +3667,12 @@
       <c r="U15" s="19"/>
     </row>
     <row r="16" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B16" s="48"/>
-      <c r="C16" s="48"/>
+      <c r="B16" s="47"/>
+      <c r="C16" s="47"/>
       <c r="D16" s="19"/>
-      <c r="E16" s="48"/>
-      <c r="F16" s="48"/>
-      <c r="G16" s="46"/>
+      <c r="E16" s="47"/>
+      <c r="F16" s="47"/>
+      <c r="G16" s="45"/>
       <c r="H16" s="19"/>
       <c r="J16" s="19"/>
       <c r="K16" s="19"/>
@@ -3642,12 +3688,12 @@
       <c r="U16" s="19"/>
     </row>
     <row r="17" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B17" s="48"/>
-      <c r="C17" s="48"/>
+      <c r="B17" s="47"/>
+      <c r="C17" s="47"/>
       <c r="D17" s="19"/>
-      <c r="E17" s="48"/>
-      <c r="F17" s="48"/>
-      <c r="G17" s="46"/>
+      <c r="E17" s="47"/>
+      <c r="F17" s="47"/>
+      <c r="G17" s="45"/>
       <c r="H17" s="19"/>
       <c r="J17" s="19"/>
       <c r="K17" s="19"/>
@@ -3663,12 +3709,12 @@
       <c r="U17" s="19"/>
     </row>
     <row r="18" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B18" s="48"/>
-      <c r="C18" s="48"/>
+      <c r="B18" s="47"/>
+      <c r="C18" s="47"/>
       <c r="D18" s="19"/>
-      <c r="E18" s="48"/>
-      <c r="F18" s="48"/>
-      <c r="G18" s="46"/>
+      <c r="E18" s="47"/>
+      <c r="F18" s="47"/>
+      <c r="G18" s="45"/>
       <c r="H18" s="19"/>
       <c r="J18" s="19"/>
       <c r="K18" s="19"/>
@@ -3684,12 +3730,12 @@
       <c r="U18" s="19"/>
     </row>
     <row r="19" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B19" s="48"/>
-      <c r="C19" s="48"/>
+      <c r="B19" s="47"/>
+      <c r="C19" s="47"/>
       <c r="D19" s="19"/>
-      <c r="E19" s="48"/>
-      <c r="F19" s="48"/>
-      <c r="G19" s="46"/>
+      <c r="E19" s="47"/>
+      <c r="F19" s="47"/>
+      <c r="G19" s="45"/>
       <c r="H19" s="19"/>
       <c r="J19" s="19"/>
       <c r="K19" s="19"/>
@@ -3705,12 +3751,12 @@
       <c r="U19" s="19"/>
     </row>
     <row r="20" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B20" s="48"/>
-      <c r="C20" s="48"/>
+      <c r="B20" s="47"/>
+      <c r="C20" s="47"/>
       <c r="D20" s="19"/>
-      <c r="E20" s="48"/>
-      <c r="F20" s="48"/>
-      <c r="G20" s="46"/>
+      <c r="E20" s="47"/>
+      <c r="F20" s="47"/>
+      <c r="G20" s="45"/>
       <c r="H20" s="19"/>
       <c r="J20" s="19"/>
       <c r="K20" s="19"/>
@@ -3726,12 +3772,12 @@
       <c r="U20" s="19"/>
     </row>
     <row r="21" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B21" s="48"/>
-      <c r="C21" s="48"/>
+      <c r="B21" s="47"/>
+      <c r="C21" s="47"/>
       <c r="D21" s="19"/>
-      <c r="E21" s="48"/>
-      <c r="F21" s="48"/>
-      <c r="G21" s="46"/>
+      <c r="E21" s="47"/>
+      <c r="F21" s="47"/>
+      <c r="G21" s="45"/>
       <c r="H21" s="19"/>
       <c r="J21" s="19"/>
       <c r="K21" s="19"/>
@@ -3747,12 +3793,12 @@
       <c r="U21" s="19"/>
     </row>
     <row r="22" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B22" s="48"/>
-      <c r="C22" s="48"/>
+      <c r="B22" s="47"/>
+      <c r="C22" s="47"/>
       <c r="D22" s="19"/>
-      <c r="E22" s="48"/>
-      <c r="F22" s="48"/>
-      <c r="G22" s="46"/>
+      <c r="E22" s="47"/>
+      <c r="F22" s="47"/>
+      <c r="G22" s="45"/>
       <c r="H22" s="19"/>
       <c r="J22" s="19"/>
       <c r="K22" s="19"/>
@@ -3768,12 +3814,12 @@
       <c r="U22" s="19"/>
     </row>
     <row r="23" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B23" s="48"/>
-      <c r="C23" s="48"/>
+      <c r="B23" s="47"/>
+      <c r="C23" s="47"/>
       <c r="D23" s="19"/>
-      <c r="E23" s="48"/>
-      <c r="F23" s="48"/>
-      <c r="G23" s="46"/>
+      <c r="E23" s="47"/>
+      <c r="F23" s="47"/>
+      <c r="G23" s="45"/>
       <c r="H23" s="19"/>
       <c r="J23" s="19"/>
       <c r="K23" s="19"/>
@@ -3789,12 +3835,12 @@
       <c r="U23" s="19"/>
     </row>
     <row r="24" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B24" s="48"/>
-      <c r="C24" s="48"/>
+      <c r="B24" s="47"/>
+      <c r="C24" s="47"/>
       <c r="D24" s="19"/>
-      <c r="E24" s="48"/>
-      <c r="F24" s="48"/>
-      <c r="G24" s="46"/>
+      <c r="E24" s="47"/>
+      <c r="F24" s="47"/>
+      <c r="G24" s="45"/>
       <c r="H24" s="19"/>
       <c r="J24" s="19"/>
       <c r="K24" s="19"/>
@@ -3810,12 +3856,12 @@
       <c r="U24" s="19"/>
     </row>
     <row r="25" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B25" s="48"/>
-      <c r="C25" s="48"/>
+      <c r="B25" s="47"/>
+      <c r="C25" s="47"/>
       <c r="D25" s="19"/>
-      <c r="E25" s="48"/>
-      <c r="F25" s="48"/>
-      <c r="G25" s="46"/>
+      <c r="E25" s="47"/>
+      <c r="F25" s="47"/>
+      <c r="G25" s="45"/>
       <c r="H25" s="19"/>
       <c r="J25" s="19"/>
       <c r="K25" s="19"/>
@@ -3831,12 +3877,12 @@
       <c r="U25" s="19"/>
     </row>
     <row r="26" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B26" s="48"/>
-      <c r="C26" s="48"/>
+      <c r="B26" s="47"/>
+      <c r="C26" s="47"/>
       <c r="D26" s="19"/>
-      <c r="E26" s="48"/>
-      <c r="F26" s="48"/>
-      <c r="G26" s="46"/>
+      <c r="E26" s="47"/>
+      <c r="F26" s="47"/>
+      <c r="G26" s="45"/>
       <c r="H26" s="19"/>
       <c r="J26" s="19"/>
       <c r="K26" s="19"/>
@@ -3856,26 +3902,26 @@
       <c r="B31" s="18"/>
     </row>
     <row r="33" spans="2:21" ht="34.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="49"/>
-      <c r="C33" s="49"/>
-      <c r="D33" s="49"/>
-      <c r="E33" s="49"/>
-      <c r="F33" s="49"/>
-      <c r="G33" s="49"/>
-      <c r="H33" s="49"/>
-      <c r="I33" s="49"/>
-      <c r="J33" s="49"/>
-      <c r="K33" s="49"/>
-      <c r="L33" s="49"/>
-      <c r="M33" s="49"/>
-      <c r="N33" s="49"/>
-      <c r="O33" s="49"/>
-      <c r="P33" s="49"/>
-      <c r="Q33" s="49"/>
-      <c r="R33" s="49"/>
-      <c r="S33" s="49"/>
-      <c r="T33" s="49"/>
-      <c r="U33" s="49"/>
+      <c r="B33" s="48"/>
+      <c r="C33" s="48"/>
+      <c r="D33" s="48"/>
+      <c r="E33" s="48"/>
+      <c r="F33" s="48"/>
+      <c r="G33" s="48"/>
+      <c r="H33" s="48"/>
+      <c r="I33" s="48"/>
+      <c r="J33" s="48"/>
+      <c r="K33" s="48"/>
+      <c r="L33" s="48"/>
+      <c r="M33" s="48"/>
+      <c r="N33" s="48"/>
+      <c r="O33" s="48"/>
+      <c r="P33" s="48"/>
+      <c r="Q33" s="48"/>
+      <c r="R33" s="48"/>
+      <c r="S33" s="48"/>
+      <c r="T33" s="48"/>
+      <c r="U33" s="48"/>
     </row>
     <row r="34" spans="2:21" ht="16" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
@@ -3899,13 +3945,13 @@
   <dimension ref="C8:K13"/>
   <sheetViews>
     <sheetView topLeftCell="A7" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="9.1640625" style="15"/>
-    <col min="3" max="3" width="14" style="15" customWidth="1"/>
+    <col min="3" max="3" width="14" style="82" customWidth="1"/>
     <col min="4" max="4" width="9.1640625" style="15"/>
     <col min="5" max="5" width="11.83203125" style="15" customWidth="1"/>
     <col min="6" max="7" width="12.1640625" style="15" customWidth="1"/>
@@ -3916,25 +3962,25 @@
   </cols>
   <sheetData>
     <row r="8" spans="3:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C8" s="17" t="s">
+      <c r="C8" s="93" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="9" spans="3:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C9" s="52"/>
-      <c r="D9" s="84" t="s">
+      <c r="C9" s="94"/>
+      <c r="D9" s="99" t="s">
         <v>81</v>
       </c>
-      <c r="E9" s="84"/>
-      <c r="F9" s="84"/>
-      <c r="G9" s="53"/>
-      <c r="H9" s="52"/>
-      <c r="I9" s="52"/>
-      <c r="J9" s="52"/>
-      <c r="K9" s="54"/>
+      <c r="E9" s="99"/>
+      <c r="F9" s="99"/>
+      <c r="G9" s="52"/>
+      <c r="H9" s="51"/>
+      <c r="I9" s="51"/>
+      <c r="J9" s="51"/>
+      <c r="K9" s="53"/>
     </row>
     <row r="10" spans="3:11" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C10" s="21" t="s">
+      <c r="C10" s="84" t="s">
         <v>122</v>
       </c>
       <c r="D10" s="22" t="s">
@@ -3958,32 +4004,32 @@
       <c r="J10" s="21" t="s">
         <v>94</v>
       </c>
-      <c r="K10" s="54"/>
+      <c r="K10" s="53"/>
     </row>
     <row r="11" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C11" s="54"/>
-      <c r="D11" s="54"/>
-      <c r="E11" s="54"/>
-      <c r="F11" s="54"/>
-      <c r="G11" s="54"/>
-      <c r="H11" s="54"/>
-      <c r="I11" s="54"/>
-      <c r="J11" s="54"/>
-      <c r="K11" s="54"/>
+      <c r="C11" s="95"/>
+      <c r="D11" s="53"/>
+      <c r="E11" s="53"/>
+      <c r="F11" s="53"/>
+      <c r="G11" s="53"/>
+      <c r="H11" s="53"/>
+      <c r="I11" s="53"/>
+      <c r="J11" s="53"/>
+      <c r="K11" s="53"/>
     </row>
     <row r="12" spans="3:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C12" s="12"/>
-      <c r="D12" s="55"/>
-      <c r="E12" s="55"/>
-      <c r="F12" s="55"/>
-      <c r="G12" s="55"/>
-      <c r="H12" s="55"/>
-      <c r="I12" s="55"/>
-      <c r="J12" s="55"/>
-      <c r="K12" s="54"/>
+      <c r="C12" s="96"/>
+      <c r="D12" s="54"/>
+      <c r="E12" s="54"/>
+      <c r="F12" s="54"/>
+      <c r="G12" s="54"/>
+      <c r="H12" s="54"/>
+      <c r="I12" s="54"/>
+      <c r="J12" s="54"/>
+      <c r="K12" s="53"/>
     </row>
     <row r="13" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="E13" s="56"/>
+      <c r="E13" s="55"/>
       <c r="F13" s="17"/>
     </row>
   </sheetData>
@@ -3996,30 +4042,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="eb4559c4-8463-4985-927f-f0d558bff8f0" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="819ae873-75e1-413b-9d00-7af9258cf281">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <Ready xmlns="819ae873-75e1-413b-9d00-7af9258cf281">true</Ready>
-    <Comments xmlns="819ae873-75e1-413b-9d00-7af9258cf281" xsi:nil="true"/>
-    <Doc_x002e_SymbolNumber xmlns="819ae873-75e1-413b-9d00-7af9258cf281" xsi:nil="true"/>
-    <_Flow_SignoffStatus xmlns="819ae873-75e1-413b-9d00-7af9258cf281" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008FB6730B0802B54A9F00C78B857E1443" ma:contentTypeVersion="21" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e7d0671dbe340d15fdce5ab7e9f4c491">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="819ae873-75e1-413b-9d00-7af9258cf281" xmlns:ns3="eb4559c4-8463-4985-927f-f0d558bff8f0" xmlns:ns4="13d80b15-5f07-43ab-b435-85767a7dac08" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2feafd61044eb4abe44eb47c2e62f3e5" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="819ae873-75e1-413b-9d00-7af9258cf281"/>
@@ -4301,38 +4323,36 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="9d8c265a-5436-43a7-80c1-713d2827ffde" ContentTypeId="0x0101" PreviousValue="false"/>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{17AB3B8A-2D8D-4EE0-964D-A16E3E636991}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="819ae873-75e1-413b-9d00-7af9258cf281"/>
-    <ds:schemaRef ds:uri="eb4559c4-8463-4985-927f-f0d558bff8f0"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="13d80b15-5f07-43ab-b435-85767a7dac08"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="eb4559c4-8463-4985-927f-f0d558bff8f0" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="819ae873-75e1-413b-9d00-7af9258cf281">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <Ready xmlns="819ae873-75e1-413b-9d00-7af9258cf281">true</Ready>
+    <Comments xmlns="819ae873-75e1-413b-9d00-7af9258cf281" xsi:nil="true"/>
+    <Doc_x002e_SymbolNumber xmlns="819ae873-75e1-413b-9d00-7af9258cf281" xsi:nil="true"/>
+    <_Flow_SignoffStatus xmlns="819ae873-75e1-413b-9d00-7af9258cf281" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9846E218-2C67-4B45-A7CB-841EE05F366A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2311233C-A90E-453E-AB6B-77EC63BE63EB}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4352,10 +4372,36 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DDE771C4-25E3-4DCA-8FB0-1AA09F9D9ED9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{17AB3B8A-2D8D-4EE0-964D-A16E3E636991}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="13d80b15-5f07-43ab-b435-85767a7dac08"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="eb4559c4-8463-4985-927f-f0d558bff8f0"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="819ae873-75e1-413b-9d00-7af9258cf281"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9846E218-2C67-4B45-A7CB-841EE05F366A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>